<commit_message>
bacground,visit counter, new lines and icons added
</commit_message>
<xml_diff>
--- a/imgs/horarios seseña.xlsx
+++ b/imgs/horarios seseña.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\web\transportes seseña\imgs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916DE51-614A-4445-9CDB-0581CFDD7597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC165C1-EA9F-4028-BAF7-19FDE499D63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>HORARIOS DE LINEA 110 URBANO SESEÑA</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>c parada en campo de futbol</t>
+  </si>
+  <si>
+    <t>Domingos y Festivos</t>
   </si>
 </sst>
 </file>
@@ -310,57 +313,12 @@
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -383,6 +341,51 @@
     <xf numFmtId="20" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -667,426 +670,426 @@
   <dimension ref="B1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="12"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="41"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="14"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="16"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="18"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="29">
+      <c r="B5" s="14">
         <v>0.25</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="15">
         <v>0.29166666666666669</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="15">
         <v>0.33680555555555558</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="15">
         <v>0.38541666666666669</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="15">
         <v>0.43055555555555558</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="15">
         <v>0.47569444444444442</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="15">
         <v>0.52083333333333337</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="15">
         <v>0.56944444444444442</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="15">
         <v>0.62152777777777779</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="26">
         <v>0.66319444444444442</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="26">
         <v>0.71180555555555547</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="26">
         <v>0.76041666666666663</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="26">
         <v>0.80902777777777779</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="26">
         <v>0.85763888888888884</v>
       </c>
-      <c r="P5" s="41">
+      <c r="P5" s="26">
         <v>0.90625</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="16">
         <v>0.95486111111111116</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
+      <c r="B6" s="17">
         <v>0.27430555555555552</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="18">
         <v>0.31597222222222221</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="18">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="18">
         <v>0.40972222222222227</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="18">
         <v>0.4548611111111111</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="18">
         <v>0.5</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="18">
         <v>0.54513888888888895</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="18">
         <v>0.59375</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="18">
         <v>0.64583333333333337</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="27">
         <v>0.6875</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="27">
         <v>0.73611111111111116</v>
       </c>
-      <c r="M6" s="42">
+      <c r="M6" s="27">
         <v>0.78472222222222221</v>
       </c>
-      <c r="N6" s="42">
+      <c r="N6" s="27">
         <v>0.83333333333333337</v>
       </c>
-      <c r="O6" s="42">
+      <c r="O6" s="27">
         <v>0.88194444444444453</v>
       </c>
-      <c r="P6" s="42">
+      <c r="P6" s="27">
         <v>0.93055555555555547</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q6" s="19">
         <v>0.97916666666666663</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="20"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="16"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="32"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
+      <c r="B9" s="22">
         <v>0.28472222222222221</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="20">
         <v>0.3298611111111111</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="28">
         <v>0.375</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="29">
         <v>0.4236111111111111</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="28">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="29">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="28">
         <v>0.56944444444444442</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="20">
         <v>0.61805555555555558</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="23">
         <v>0.66319444444444442</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="20">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="23">
         <v>0.75347222222222221</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="20">
         <v>0.79861111111111116</v>
       </c>
-      <c r="N9" s="38">
+      <c r="N9" s="23">
         <v>0.84375</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="20">
         <v>0.88888888888888884</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="23">
         <v>0.93402777777777779</v>
       </c>
-      <c r="Q9" s="36">
+      <c r="Q9" s="21">
         <v>0.97916666666666663</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="22"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="35"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="16"/>
+      <c r="B11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="32"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="32">
+      <c r="B12" s="17">
         <v>0.3298611111111111</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="24">
         <v>0.375</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="18">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="24">
         <v>0.47222222222222227</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="18">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="24">
         <v>0.56944444444444442</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="18">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="24">
         <v>0.66319444444444442</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="18">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="24">
         <v>0.75347222222222221</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="18">
         <v>0.79861111111111116</v>
       </c>
-      <c r="M12" s="39">
+      <c r="M12" s="24">
         <v>0.84375</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="18">
         <v>0.88888888888888884</v>
       </c>
-      <c r="O12" s="39">
+      <c r="O12" s="24">
         <v>0.93402777777777779</v>
       </c>
-      <c r="P12" s="33">
+      <c r="P12" s="18">
         <v>0.97916666666666663</v>
       </c>
-      <c r="Q12" s="23"/>
+      <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="18"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="7" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="25"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="28"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>